<commit_message>
Update date format for adm_date
</commit_message>
<xml_diff>
--- a/data_processing_elements-DSE.xlsx
+++ b/data_processing_elements-DSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8989DCEF-0B06-4238-B8EE-B9090599C27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A322B955-7833-46E2-8611-E5AB17C3A16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1911,7 +1911,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>